<commit_message>
Rename script files with sequential order
</commit_message>
<xml_diff>
--- a/results/resultsParticipant.xlsx
+++ b/results/resultsParticipant.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,16 +417,396 @@
         <v>3000</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>6.60869307700319</v>
+      </c>
+      <c r="F2">
+        <v>1070.6317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3000</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>7.299787708709571</v>
+      </c>
+      <c r="F3">
+        <v>1415.9084</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>7.85893764337613</v>
+      </c>
+      <c r="F4">
+        <v>642.5690000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3000</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>4.593158806225821</v>
+      </c>
+      <c r="F5">
+        <v>877.062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3000</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>5.17807708575072</v>
+      </c>
+      <c r="F6">
+        <v>728.8030999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>3000</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>4.725605545853591</v>
+      </c>
+      <c r="F7">
+        <v>873.9599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3000</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>5.333819297697558</v>
+      </c>
+      <c r="F8">
+        <v>1330.8975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3000</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>5.108525760744161</v>
+      </c>
+      <c r="F9">
+        <v>600.6339999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3000</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>7.377457297111516</v>
+      </c>
+      <c r="F10">
+        <v>755.0204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3000</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>6.738185545039576</v>
+      </c>
+      <c r="F11">
+        <v>1522.4909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3000</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>6.018201625009492</v>
+      </c>
+      <c r="F12">
+        <v>1863.4546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>3000</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>7.005961915086409</v>
+      </c>
+      <c r="F13">
+        <v>255.7185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>3000</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>5.040659110120907</v>
+      </c>
+      <c r="F14">
+        <v>1565.5031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>3000</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>3.597975746048344</v>
+      </c>
+      <c r="F15">
+        <v>1179.2965</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>3000</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>4.420036612820993</v>
+      </c>
+      <c r="F16">
+        <v>803.2319000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>3000</v>
+      </c>
+      <c r="C17">
         <v>16</v>
       </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17">
         <v>4.464905601109714</v>
       </c>
-      <c r="F2">
+      <c r="F17">
         <v>800.5603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>3000</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>5.116316240997665</v>
+      </c>
+      <c r="F18">
+        <v>1236.5861</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>3000</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>2.906358479492045</v>
+      </c>
+      <c r="F19">
+        <v>1097.7146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>3000</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>4.777966849038944</v>
+      </c>
+      <c r="F20">
+        <v>1559.909399999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>3000</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>4.387744588261096</v>
+      </c>
+      <c r="F21">
+        <v>779.5659999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>